<commit_message>
Fixed overwriting an excel file
</commit_message>
<xml_diff>
--- a/report_creation_program/report_creation_program/bin/Debug/SalesReport.xlsx
+++ b/report_creation_program/report_creation_program/bin/Debug/SalesReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\College Homework\CAPSTONE\report_creation_program\report_creation_program\report_creation_program\report_creation_program\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{60B425B4-C823-4C0D-AA76-06E9A6A11BC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{928C7F4D-F6E6-44C8-B4E7-055F58EDAA50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15450" yWindow="1095" windowWidth="13350" windowHeight="11835" xr2:uid="{98B64D7C-C433-4A26-90AD-1EE8344833FB}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" xr2:uid="{063E4F0E-0B3B-478F-A1F2-9A7F6F584C4D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
-    <t>Sales for the last year (365 days)</t>
+    <t>Sales for the last day</t>
   </si>
   <si>
     <t>Medals</t>
@@ -429,7 +429,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E07001E-617E-4195-86AD-E4FFA63A1202}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AE1B7A7-E841-4DE4-A5B0-843300885EA6}">
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -487,13 +487,13 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>49.75</v>
+        <v>0</v>
       </c>
       <c r="B3">
-        <v>60.97</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>16.5</v>
+        <v>0</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -505,7 +505,7 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>74.75</v>
+        <v>0</v>
       </c>
       <c r="H3">
         <v>0</v>

</xml_diff>

<commit_message>
Prettied up report creation tool
</commit_message>
<xml_diff>
--- a/report_creation_program/report_creation_program/bin/Debug/SalesReport.xlsx
+++ b/report_creation_program/report_creation_program/bin/Debug/SalesReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\College Homework\CAPSTONE\report_creation_program\report_creation_program\report_creation_program\report_creation_program\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6989485F-80D9-44B0-ACE7-F0F2660DBDA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1DE445A1-F3F0-4700-BF4E-40B3C0F1A34F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" xr2:uid="{B4938B14-FC98-42C2-9C16-C814952ED0F1}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" xr2:uid="{62BE7923-426E-41E8-AB05-DF7052ED05D4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
-    <t>Sales for the last year (365 days)</t>
+    <t>Sales for the last day</t>
   </si>
   <si>
     <t>Medals</t>
@@ -429,7 +429,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{784291F4-110F-489D-89FD-507BBCFE38B6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5696148B-2F8C-41CA-98D0-F0A38EA152AC}">
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -487,13 +487,13 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>49.75</v>
+        <v>0</v>
       </c>
       <c r="B3">
-        <v>60.97</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>16.5</v>
+        <v>0</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -505,7 +505,7 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>74.75</v>
+        <v>0</v>
       </c>
       <c r="H3">
         <v>0</v>

</xml_diff>

<commit_message>
Changed assembly name to ReportCreation
</commit_message>
<xml_diff>
--- a/report_creation_program/report_creation_program/bin/Debug/SalesReport.xlsx
+++ b/report_creation_program/report_creation_program/bin/Debug/SalesReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\College Homework\CAPSTONE\report_creation_program\report_creation_program\report_creation_program\report_creation_program\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1DE445A1-F3F0-4700-BF4E-40B3C0F1A34F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E87C9612-B3B5-48F7-BBF0-7233E582A331}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" xr2:uid="{62BE7923-426E-41E8-AB05-DF7052ED05D4}"/>
+    <workbookView xWindow="31050" yWindow="2460" windowWidth="21600" windowHeight="11385" xr2:uid="{C89B81C4-346E-4B73-912E-5CFDBE794343}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -429,7 +429,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5696148B-2F8C-41CA-98D0-F0A38EA152AC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08EF62E7-E269-4022-8FC4-081E0C6AC64B}">
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Better handling of connection loss
</commit_message>
<xml_diff>
--- a/report_creation_program/report_creation_program/bin/Debug/SalesReport.xlsx
+++ b/report_creation_program/report_creation_program/bin/Debug/SalesReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\College Homework\CAPSTONE\report_creation_program\report_creation_program\report_creation_program\report_creation_program\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E87C9612-B3B5-48F7-BBF0-7233E582A331}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F59F77F4-2E3C-499B-8126-E3B1BDFAE438}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31050" yWindow="2460" windowWidth="21600" windowHeight="11385" xr2:uid="{C89B81C4-346E-4B73-912E-5CFDBE794343}"/>
+    <workbookView xWindow="31395" yWindow="2805" windowWidth="21600" windowHeight="11385" xr2:uid="{18CEED30-6C45-4D61-AE7B-C54024A76F7B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -429,7 +429,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08EF62E7-E269-4022-8FC4-081E0C6AC64B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39FF24B2-419A-44BB-80C3-2C3F8F9A51DC}">
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Fixed sales report so the view pulls from the correct tables. Also added bugfix to stop 'in use by another process' errors. Changed email title to 'Sales Report' instead of 'test'
</commit_message>
<xml_diff>
--- a/report_creation_program/report_creation_program/bin/Debug/SalesReport.xlsx
+++ b/report_creation_program/report_creation_program/bin/Debug/SalesReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\College Homework\CAPSTONE\report_creation_program\report_creation_program\report_creation_program\bin\Debug\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/016be9303c01b4f8/Documents/SCHOOL STUFF/05 Summer 2021/Capstone/malloyethan11/report_creation_program/report_creation_program/report_creation_program/bin/Debug/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AFF5061E-DA56-466E-886B-C3348843A409}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{22E0ADA0-2075-4557-B836-FA27DD98DD31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44250" yWindow="1275" windowWidth="13350" windowHeight="11835" xr2:uid="{66940968-C0B1-42D0-9343-0028903B9E93}"/>
+    <workbookView xWindow="-26490" yWindow="1005" windowWidth="22980" windowHeight="13770" xr2:uid="{F4131783-BFE1-4D6F-9080-F1D4D0F9195C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
-    <t>Sales for the last week</t>
+    <t>Sales for the last year (365 days)</t>
   </si>
   <si>
     <t>Medals</t>
@@ -429,7 +429,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA977109-1D89-40C3-987B-10A056354FE0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4029B001-F8F6-474C-9F8C-32DDF2256442}">
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -487,25 +487,25 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>0</v>
+        <v>100.4</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>1520.91</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>9.9499999999999993</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>24.95</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>492.75</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -517,10 +517,10 @@
         <v>0</v>
       </c>
       <c r="K3">
-        <v>0</v>
+        <v>7.9</v>
       </c>
       <c r="L3">
-        <v>0</v>
+        <v>48.9</v>
       </c>
       <c r="M3">
         <v>0</v>

</xml_diff>